<commit_message>
power analysis added to all paradigms
</commit_message>
<xml_diff>
--- a/Longitudinal_induction_analysis/EPM/EPM_binned_longitudinal_data.xlsx
+++ b/Longitudinal_induction_analysis/EPM/EPM_binned_longitudinal_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11207"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10315"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/annastuckert/Documents/GitHub/TDPBehaviorAnalysis/Longitudinal_induction_analysis/EPM/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CBC777A-5DB0-0949-ABE7-FC1B35254F47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B0AA570-1771-2A4D-99D1-CA5821E55FC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2680" yWindow="500" windowWidth="14700" windowHeight="15180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="14700" windowHeight="15180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Analysis" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="36">
   <si>
     <t>Distance moved</t>
   </si>
@@ -107,6 +107,27 @@
   </si>
   <si>
     <t>Timebin 2</t>
+  </si>
+  <si>
+    <t>247</t>
+  </si>
+  <si>
+    <t>224</t>
+  </si>
+  <si>
+    <t>250</t>
+  </si>
+  <si>
+    <t>256</t>
+  </si>
+  <si>
+    <t>262</t>
+  </si>
+  <si>
+    <t>271</t>
+  </si>
+  <si>
+    <t>281</t>
   </si>
 </sst>
 </file>
@@ -449,10 +470,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O49"/>
+  <dimension ref="A1:O91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="F40" sqref="F40"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="B50" sqref="B50:B91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2763,6 +2784,1980 @@
         <v>16</v>
       </c>
     </row>
+    <row r="50" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>29</v>
+      </c>
+      <c r="B50" t="s">
+        <v>27</v>
+      </c>
+      <c r="C50">
+        <v>1213.28</v>
+      </c>
+      <c r="D50">
+        <v>4.0646000000000004</v>
+      </c>
+      <c r="E50">
+        <v>9</v>
+      </c>
+      <c r="F50">
+        <v>27.42</v>
+      </c>
+      <c r="G50">
+        <v>6</v>
+      </c>
+      <c r="H50">
+        <v>9.58</v>
+      </c>
+      <c r="I50">
+        <v>10</v>
+      </c>
+      <c r="J50">
+        <v>90.82</v>
+      </c>
+      <c r="K50">
+        <v>16</v>
+      </c>
+      <c r="L50">
+        <v>103.16</v>
+      </c>
+      <c r="M50">
+        <v>40</v>
+      </c>
+      <c r="N50">
+        <v>67.98</v>
+      </c>
+      <c r="O50" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="51" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>29</v>
+      </c>
+      <c r="B51" t="s">
+        <v>28</v>
+      </c>
+      <c r="C51">
+        <v>992.24900000000002</v>
+      </c>
+      <c r="D51">
+        <v>3.3092600000000001</v>
+      </c>
+      <c r="E51">
+        <v>7</v>
+      </c>
+      <c r="F51">
+        <v>26.12</v>
+      </c>
+      <c r="G51">
+        <v>13</v>
+      </c>
+      <c r="H51">
+        <v>31.5</v>
+      </c>
+      <c r="I51">
+        <v>9</v>
+      </c>
+      <c r="J51">
+        <v>92.2</v>
+      </c>
+      <c r="K51">
+        <v>10</v>
+      </c>
+      <c r="L51">
+        <v>86.98</v>
+      </c>
+      <c r="M51">
+        <v>38</v>
+      </c>
+      <c r="N51">
+        <v>63.2</v>
+      </c>
+      <c r="O51" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="52" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>30</v>
+      </c>
+      <c r="B52" t="s">
+        <v>27</v>
+      </c>
+      <c r="C52">
+        <v>1077.3499999999999</v>
+      </c>
+      <c r="D52">
+        <v>3.6024600000000002</v>
+      </c>
+      <c r="E52">
+        <v>7</v>
+      </c>
+      <c r="F52">
+        <v>16.68</v>
+      </c>
+      <c r="G52">
+        <v>4</v>
+      </c>
+      <c r="H52">
+        <v>4.26</v>
+      </c>
+      <c r="I52">
+        <v>14</v>
+      </c>
+      <c r="J52">
+        <v>144.47999999999999</v>
+      </c>
+      <c r="K52">
+        <v>11</v>
+      </c>
+      <c r="L52">
+        <v>91.66</v>
+      </c>
+      <c r="M52">
+        <v>34</v>
+      </c>
+      <c r="N52">
+        <v>42.52</v>
+      </c>
+      <c r="O52" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="53" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>30</v>
+      </c>
+      <c r="B53" t="s">
+        <v>28</v>
+      </c>
+      <c r="C53">
+        <v>811.37699999999995</v>
+      </c>
+      <c r="D53">
+        <v>2.7074799999999999</v>
+      </c>
+      <c r="E53">
+        <v>8</v>
+      </c>
+      <c r="F53">
+        <v>43.34</v>
+      </c>
+      <c r="G53">
+        <v>3</v>
+      </c>
+      <c r="H53">
+        <v>26.1</v>
+      </c>
+      <c r="I53">
+        <v>2</v>
+      </c>
+      <c r="J53">
+        <v>24.66</v>
+      </c>
+      <c r="K53">
+        <v>8</v>
+      </c>
+      <c r="L53">
+        <v>167.32</v>
+      </c>
+      <c r="M53">
+        <v>20</v>
+      </c>
+      <c r="N53">
+        <v>38.5</v>
+      </c>
+      <c r="O53" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="54" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>29</v>
+      </c>
+      <c r="B54" t="s">
+        <v>27</v>
+      </c>
+      <c r="C54">
+        <v>1080.47</v>
+      </c>
+      <c r="D54">
+        <v>3.6021899999999998</v>
+      </c>
+      <c r="E54">
+        <v>2</v>
+      </c>
+      <c r="F54">
+        <v>5.58162</v>
+      </c>
+      <c r="G54">
+        <v>2</v>
+      </c>
+      <c r="H54">
+        <v>2.24065</v>
+      </c>
+      <c r="I54">
+        <v>8</v>
+      </c>
+      <c r="J54">
+        <v>143.27500000000001</v>
+      </c>
+      <c r="K54">
+        <v>10</v>
+      </c>
+      <c r="L54">
+        <v>118.914</v>
+      </c>
+      <c r="M54">
+        <v>20</v>
+      </c>
+      <c r="N54">
+        <v>29.968699999999998</v>
+      </c>
+      <c r="O54" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="55" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>29</v>
+      </c>
+      <c r="B55" t="s">
+        <v>28</v>
+      </c>
+      <c r="C55">
+        <v>1060.8800000000001</v>
+      </c>
+      <c r="D55">
+        <v>3.5361699999999998</v>
+      </c>
+      <c r="E55">
+        <v>6</v>
+      </c>
+      <c r="F55">
+        <v>33.409700000000001</v>
+      </c>
+      <c r="G55">
+        <v>2</v>
+      </c>
+      <c r="H55">
+        <v>7.8422700000000001</v>
+      </c>
+      <c r="I55">
+        <v>23</v>
+      </c>
+      <c r="J55">
+        <v>76.709199999999996</v>
+      </c>
+      <c r="K55">
+        <v>10</v>
+      </c>
+      <c r="L55">
+        <v>145.22800000000001</v>
+      </c>
+      <c r="M55">
+        <v>38</v>
+      </c>
+      <c r="N55">
+        <v>36.810699999999997</v>
+      </c>
+      <c r="O55" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="56" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>30</v>
+      </c>
+      <c r="B56" t="s">
+        <v>27</v>
+      </c>
+      <c r="C56">
+        <v>813.07299999999998</v>
+      </c>
+      <c r="D56">
+        <v>2.7119900000000001</v>
+      </c>
+      <c r="E56">
+        <v>2</v>
+      </c>
+      <c r="F56">
+        <v>1.9605699999999999</v>
+      </c>
+      <c r="G56">
+        <v>3</v>
+      </c>
+      <c r="H56">
+        <v>12.4236</v>
+      </c>
+      <c r="I56">
+        <v>1</v>
+      </c>
+      <c r="J56">
+        <v>10.375999999999999</v>
+      </c>
+      <c r="K56">
+        <v>7</v>
+      </c>
+      <c r="L56">
+        <v>259.13499999999999</v>
+      </c>
+      <c r="M56">
+        <v>12</v>
+      </c>
+      <c r="N56">
+        <v>16.104700000000001</v>
+      </c>
+      <c r="O56" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="57" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>30</v>
+      </c>
+      <c r="B57" t="s">
+        <v>28</v>
+      </c>
+      <c r="C57">
+        <v>1051.79</v>
+      </c>
+      <c r="D57">
+        <v>3.5098500000000001</v>
+      </c>
+      <c r="E57">
+        <v>11</v>
+      </c>
+      <c r="F57">
+        <v>42.932400000000001</v>
+      </c>
+      <c r="G57">
+        <v>2</v>
+      </c>
+      <c r="H57">
+        <v>5.3615500000000003</v>
+      </c>
+      <c r="I57">
+        <v>5</v>
+      </c>
+      <c r="J57">
+        <v>122.389</v>
+      </c>
+      <c r="K57">
+        <v>9</v>
+      </c>
+      <c r="L57">
+        <v>96.928100000000001</v>
+      </c>
+      <c r="M57">
+        <v>23</v>
+      </c>
+      <c r="N57">
+        <v>32.109299999999998</v>
+      </c>
+      <c r="O57" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="58" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>29</v>
+      </c>
+      <c r="B58" t="s">
+        <v>27</v>
+      </c>
+      <c r="C58">
+        <v>1339.74</v>
+      </c>
+      <c r="D58">
+        <v>4.4690599999999998</v>
+      </c>
+      <c r="E58">
+        <v>9</v>
+      </c>
+      <c r="F58">
+        <v>37.6</v>
+      </c>
+      <c r="G58">
+        <v>16</v>
+      </c>
+      <c r="H58">
+        <v>66.08</v>
+      </c>
+      <c r="I58">
+        <v>1</v>
+      </c>
+      <c r="J58">
+        <v>9.74</v>
+      </c>
+      <c r="K58">
+        <v>19</v>
+      </c>
+      <c r="L58">
+        <v>89.46</v>
+      </c>
+      <c r="M58">
+        <v>44</v>
+      </c>
+      <c r="N58">
+        <v>97.12</v>
+      </c>
+      <c r="O58" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="59" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>29</v>
+      </c>
+      <c r="B59" t="s">
+        <v>28</v>
+      </c>
+      <c r="C59">
+        <v>1580.23</v>
+      </c>
+      <c r="D59">
+        <v>5.3278100000000004</v>
+      </c>
+      <c r="E59">
+        <v>14</v>
+      </c>
+      <c r="F59">
+        <v>81.48</v>
+      </c>
+      <c r="G59">
+        <v>19</v>
+      </c>
+      <c r="H59">
+        <v>78.540000000000006</v>
+      </c>
+      <c r="I59">
+        <v>10</v>
+      </c>
+      <c r="J59">
+        <v>27.7</v>
+      </c>
+      <c r="K59">
+        <v>10</v>
+      </c>
+      <c r="L59">
+        <v>34.18</v>
+      </c>
+      <c r="M59">
+        <v>47</v>
+      </c>
+      <c r="N59">
+        <v>75.260000000000005</v>
+      </c>
+      <c r="O59" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="60" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>30</v>
+      </c>
+      <c r="B60" t="s">
+        <v>27</v>
+      </c>
+      <c r="C60">
+        <v>787.92200000000003</v>
+      </c>
+      <c r="D60">
+        <v>2.6274000000000002</v>
+      </c>
+      <c r="E60">
+        <v>10</v>
+      </c>
+      <c r="F60">
+        <v>7.2821100000000003</v>
+      </c>
+      <c r="G60">
+        <v>1</v>
+      </c>
+      <c r="H60">
+        <v>0.28008100000000002</v>
+      </c>
+      <c r="I60">
+        <v>11</v>
+      </c>
+      <c r="J60">
+        <v>225.86500000000001</v>
+      </c>
+      <c r="K60">
+        <v>2</v>
+      </c>
+      <c r="L60">
+        <v>30.6219</v>
+      </c>
+      <c r="M60">
+        <v>23</v>
+      </c>
+      <c r="N60">
+        <v>35.950400000000002</v>
+      </c>
+      <c r="O60" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="61" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>30</v>
+      </c>
+      <c r="B61" t="s">
+        <v>28</v>
+      </c>
+      <c r="C61">
+        <v>921.46699999999998</v>
+      </c>
+      <c r="D61">
+        <v>3.0718899999999998</v>
+      </c>
+      <c r="E61">
+        <v>7</v>
+      </c>
+      <c r="F61">
+        <v>25.727499999999999</v>
+      </c>
+      <c r="G61">
+        <v>3</v>
+      </c>
+      <c r="H61">
+        <v>9.2887400000000007</v>
+      </c>
+      <c r="I61">
+        <v>5</v>
+      </c>
+      <c r="J61">
+        <v>121.215</v>
+      </c>
+      <c r="K61">
+        <v>8</v>
+      </c>
+      <c r="L61">
+        <v>86.992199999999997</v>
+      </c>
+      <c r="M61">
+        <v>22</v>
+      </c>
+      <c r="N61">
+        <v>56.776499999999999</v>
+      </c>
+      <c r="O61" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="62" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>31</v>
+      </c>
+      <c r="B62" t="s">
+        <v>27</v>
+      </c>
+      <c r="C62">
+        <v>775.61500000000001</v>
+      </c>
+      <c r="D62">
+        <v>2.5997699999999999</v>
+      </c>
+      <c r="E62">
+        <v>2</v>
+      </c>
+      <c r="F62">
+        <v>3.46</v>
+      </c>
+      <c r="G62">
+        <v>8</v>
+      </c>
+      <c r="H62">
+        <v>29.28</v>
+      </c>
+      <c r="I62">
+        <v>16</v>
+      </c>
+      <c r="J62">
+        <v>200.64</v>
+      </c>
+      <c r="K62">
+        <v>2</v>
+      </c>
+      <c r="L62">
+        <v>14.68</v>
+      </c>
+      <c r="M62">
+        <v>26</v>
+      </c>
+      <c r="N62">
+        <v>50.56</v>
+      </c>
+      <c r="O62" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="63" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>31</v>
+      </c>
+      <c r="B63" t="s">
+        <v>28</v>
+      </c>
+      <c r="C63">
+        <v>815.99800000000005</v>
+      </c>
+      <c r="D63">
+        <v>2.7214399999999999</v>
+      </c>
+      <c r="E63">
+        <v>6</v>
+      </c>
+      <c r="F63">
+        <v>35.46</v>
+      </c>
+      <c r="G63">
+        <v>9</v>
+      </c>
+      <c r="H63">
+        <v>30.12</v>
+      </c>
+      <c r="I63">
+        <v>6</v>
+      </c>
+      <c r="J63">
+        <v>65.78</v>
+      </c>
+      <c r="K63">
+        <v>13</v>
+      </c>
+      <c r="L63">
+        <v>74.2</v>
+      </c>
+      <c r="M63">
+        <v>33</v>
+      </c>
+      <c r="N63">
+        <v>94.44</v>
+      </c>
+      <c r="O63" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="64" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>32</v>
+      </c>
+      <c r="B64" t="s">
+        <v>27</v>
+      </c>
+      <c r="C64">
+        <v>851.97799999999995</v>
+      </c>
+      <c r="D64">
+        <v>2.8420100000000001</v>
+      </c>
+      <c r="E64">
+        <v>3</v>
+      </c>
+      <c r="F64">
+        <v>12.72</v>
+      </c>
+      <c r="G64">
+        <v>4</v>
+      </c>
+      <c r="H64">
+        <v>14.14</v>
+      </c>
+      <c r="I64">
+        <v>6</v>
+      </c>
+      <c r="J64">
+        <v>144.32</v>
+      </c>
+      <c r="K64">
+        <v>8</v>
+      </c>
+      <c r="L64">
+        <v>73.959999999999994</v>
+      </c>
+      <c r="M64">
+        <v>20</v>
+      </c>
+      <c r="N64">
+        <v>54.86</v>
+      </c>
+      <c r="O64" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="65" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>32</v>
+      </c>
+      <c r="B65" t="s">
+        <v>28</v>
+      </c>
+      <c r="C65">
+        <v>667.29399999999998</v>
+      </c>
+      <c r="D65">
+        <v>2.2254999999999998</v>
+      </c>
+      <c r="E65">
+        <v>0</v>
+      </c>
+      <c r="F65">
+        <v>0</v>
+      </c>
+      <c r="G65">
+        <v>4</v>
+      </c>
+      <c r="H65">
+        <v>14.18</v>
+      </c>
+      <c r="I65">
+        <v>6</v>
+      </c>
+      <c r="J65">
+        <v>91.16</v>
+      </c>
+      <c r="K65">
+        <v>4</v>
+      </c>
+      <c r="L65">
+        <v>158.32</v>
+      </c>
+      <c r="M65">
+        <v>14</v>
+      </c>
+      <c r="N65">
+        <v>36.340000000000003</v>
+      </c>
+      <c r="O65" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="66" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>33</v>
+      </c>
+      <c r="B66" t="s">
+        <v>27</v>
+      </c>
+      <c r="C66">
+        <v>919.327</v>
+      </c>
+      <c r="D66">
+        <v>3.0829200000000001</v>
+      </c>
+      <c r="E66">
+        <v>15</v>
+      </c>
+      <c r="F66">
+        <v>68.12</v>
+      </c>
+      <c r="G66">
+        <v>7</v>
+      </c>
+      <c r="H66">
+        <v>21.86</v>
+      </c>
+      <c r="I66">
+        <v>1</v>
+      </c>
+      <c r="J66">
+        <v>7.42</v>
+      </c>
+      <c r="K66">
+        <v>12</v>
+      </c>
+      <c r="L66">
+        <v>120.92</v>
+      </c>
+      <c r="M66">
+        <v>35</v>
+      </c>
+      <c r="N66">
+        <v>80.180000000000007</v>
+      </c>
+      <c r="O66" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="67" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>33</v>
+      </c>
+      <c r="B67" t="s">
+        <v>28</v>
+      </c>
+      <c r="C67">
+        <v>526.78599999999994</v>
+      </c>
+      <c r="D67">
+        <v>1.7568900000000001</v>
+      </c>
+      <c r="E67">
+        <v>1</v>
+      </c>
+      <c r="F67">
+        <v>3.44</v>
+      </c>
+      <c r="G67">
+        <v>0</v>
+      </c>
+      <c r="H67">
+        <v>0</v>
+      </c>
+      <c r="I67">
+        <v>3</v>
+      </c>
+      <c r="J67">
+        <v>30.54</v>
+      </c>
+      <c r="K67">
+        <v>6</v>
+      </c>
+      <c r="L67">
+        <v>216.9</v>
+      </c>
+      <c r="M67">
+        <v>9</v>
+      </c>
+      <c r="N67">
+        <v>49.12</v>
+      </c>
+      <c r="O67" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="68" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>34</v>
+      </c>
+      <c r="B68" t="s">
+        <v>27</v>
+      </c>
+      <c r="C68">
+        <v>721.74199999999996</v>
+      </c>
+      <c r="D68">
+        <v>2.4075700000000002</v>
+      </c>
+      <c r="E68">
+        <v>2</v>
+      </c>
+      <c r="F68">
+        <v>10.82</v>
+      </c>
+      <c r="G68">
+        <v>4</v>
+      </c>
+      <c r="H68">
+        <v>5.6</v>
+      </c>
+      <c r="I68">
+        <v>8</v>
+      </c>
+      <c r="J68">
+        <v>135.4</v>
+      </c>
+      <c r="K68">
+        <v>2</v>
+      </c>
+      <c r="L68">
+        <v>130.84</v>
+      </c>
+      <c r="M68">
+        <v>15</v>
+      </c>
+      <c r="N68">
+        <v>17.34</v>
+      </c>
+      <c r="O68" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="69" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
+        <v>34</v>
+      </c>
+      <c r="B69" t="s">
+        <v>28</v>
+      </c>
+      <c r="C69">
+        <v>539.178</v>
+      </c>
+      <c r="D69">
+        <v>1.7982199999999999</v>
+      </c>
+      <c r="E69">
+        <v>3</v>
+      </c>
+      <c r="F69">
+        <v>34.46</v>
+      </c>
+      <c r="G69">
+        <v>0</v>
+      </c>
+      <c r="H69">
+        <v>0</v>
+      </c>
+      <c r="I69">
+        <v>8</v>
+      </c>
+      <c r="J69">
+        <v>183.08</v>
+      </c>
+      <c r="K69">
+        <v>3</v>
+      </c>
+      <c r="L69">
+        <v>66.900000000000006</v>
+      </c>
+      <c r="M69">
+        <v>14</v>
+      </c>
+      <c r="N69">
+        <v>15.56</v>
+      </c>
+      <c r="O69" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="70" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
+        <v>35</v>
+      </c>
+      <c r="B70" t="s">
+        <v>27</v>
+      </c>
+      <c r="C70">
+        <v>1132.4100000000001</v>
+      </c>
+      <c r="D70">
+        <v>3.77948</v>
+      </c>
+      <c r="E70">
+        <v>9</v>
+      </c>
+      <c r="F70">
+        <v>67.14</v>
+      </c>
+      <c r="G70">
+        <v>6</v>
+      </c>
+      <c r="H70">
+        <v>50.4</v>
+      </c>
+      <c r="I70">
+        <v>2</v>
+      </c>
+      <c r="J70">
+        <v>59.94</v>
+      </c>
+      <c r="K70">
+        <v>8</v>
+      </c>
+      <c r="L70">
+        <v>99.34</v>
+      </c>
+      <c r="M70">
+        <v>24</v>
+      </c>
+      <c r="N70">
+        <v>23.16</v>
+      </c>
+      <c r="O70" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="71" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
+        <v>35</v>
+      </c>
+      <c r="B71" t="s">
+        <v>28</v>
+      </c>
+      <c r="C71">
+        <v>1391.44</v>
+      </c>
+      <c r="D71">
+        <v>4.6406000000000001</v>
+      </c>
+      <c r="E71">
+        <v>9</v>
+      </c>
+      <c r="F71">
+        <v>83.68</v>
+      </c>
+      <c r="G71">
+        <v>13</v>
+      </c>
+      <c r="H71">
+        <v>55.38</v>
+      </c>
+      <c r="I71">
+        <v>9</v>
+      </c>
+      <c r="J71">
+        <v>58.42</v>
+      </c>
+      <c r="K71">
+        <v>10</v>
+      </c>
+      <c r="L71">
+        <v>68.08</v>
+      </c>
+      <c r="M71">
+        <v>40</v>
+      </c>
+      <c r="N71">
+        <v>34.44</v>
+      </c>
+      <c r="O71" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="72" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
+        <v>31</v>
+      </c>
+      <c r="B72" t="s">
+        <v>27</v>
+      </c>
+      <c r="C72">
+        <v>781.37900000000002</v>
+      </c>
+      <c r="D72">
+        <v>2.6086</v>
+      </c>
+      <c r="E72">
+        <v>6</v>
+      </c>
+      <c r="F72">
+        <v>14.96</v>
+      </c>
+      <c r="G72">
+        <v>4</v>
+      </c>
+      <c r="H72">
+        <v>3.12</v>
+      </c>
+      <c r="I72">
+        <v>10</v>
+      </c>
+      <c r="J72">
+        <v>225.54</v>
+      </c>
+      <c r="K72">
+        <v>2</v>
+      </c>
+      <c r="L72">
+        <v>29.3</v>
+      </c>
+      <c r="M72">
+        <v>21</v>
+      </c>
+      <c r="N72">
+        <v>26.64</v>
+      </c>
+      <c r="O72" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="73" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
+        <v>31</v>
+      </c>
+      <c r="B73" t="s">
+        <v>28</v>
+      </c>
+      <c r="C73">
+        <v>1183.58</v>
+      </c>
+      <c r="D73">
+        <v>3.9473699999999998</v>
+      </c>
+      <c r="E73">
+        <v>10</v>
+      </c>
+      <c r="F73">
+        <v>45.98</v>
+      </c>
+      <c r="G73">
+        <v>4</v>
+      </c>
+      <c r="H73">
+        <v>15.9</v>
+      </c>
+      <c r="I73">
+        <v>12</v>
+      </c>
+      <c r="J73">
+        <v>110.06</v>
+      </c>
+      <c r="K73">
+        <v>10</v>
+      </c>
+      <c r="L73">
+        <v>65.540000000000006</v>
+      </c>
+      <c r="M73">
+        <v>35</v>
+      </c>
+      <c r="N73">
+        <v>62.52</v>
+      </c>
+      <c r="O73" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="74" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
+        <v>32</v>
+      </c>
+      <c r="B74" t="s">
+        <v>27</v>
+      </c>
+      <c r="C74">
+        <v>794.73</v>
+      </c>
+      <c r="D74">
+        <v>2.6510400000000001</v>
+      </c>
+      <c r="E74">
+        <v>0</v>
+      </c>
+      <c r="F74">
+        <v>0</v>
+      </c>
+      <c r="G74">
+        <v>0</v>
+      </c>
+      <c r="H74">
+        <v>0</v>
+      </c>
+      <c r="I74">
+        <v>9</v>
+      </c>
+      <c r="J74">
+        <v>212.82</v>
+      </c>
+      <c r="K74">
+        <v>4</v>
+      </c>
+      <c r="L74">
+        <v>72.94</v>
+      </c>
+      <c r="M74">
+        <v>11</v>
+      </c>
+      <c r="N74">
+        <v>14.08</v>
+      </c>
+      <c r="O74" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="75" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A75" t="s">
+        <v>32</v>
+      </c>
+      <c r="B75" t="s">
+        <v>28</v>
+      </c>
+      <c r="C75">
+        <v>821.42700000000002</v>
+      </c>
+      <c r="D75">
+        <v>2.7395499999999999</v>
+      </c>
+      <c r="E75">
+        <v>2</v>
+      </c>
+      <c r="F75">
+        <v>16.12</v>
+      </c>
+      <c r="G75">
+        <v>1</v>
+      </c>
+      <c r="H75">
+        <v>3.68</v>
+      </c>
+      <c r="I75">
+        <v>6</v>
+      </c>
+      <c r="J75">
+        <v>121.46</v>
+      </c>
+      <c r="K75">
+        <v>8</v>
+      </c>
+      <c r="L75">
+        <v>133.78</v>
+      </c>
+      <c r="M75">
+        <v>15</v>
+      </c>
+      <c r="N75">
+        <v>24.96</v>
+      </c>
+      <c r="O75" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="76" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
+        <v>33</v>
+      </c>
+      <c r="B76" t="s">
+        <v>27</v>
+      </c>
+      <c r="C76">
+        <v>972.12599999999998</v>
+      </c>
+      <c r="D76">
+        <v>3.2471299999999998</v>
+      </c>
+      <c r="E76">
+        <v>7</v>
+      </c>
+      <c r="F76">
+        <v>16.84</v>
+      </c>
+      <c r="G76">
+        <v>2</v>
+      </c>
+      <c r="H76">
+        <v>10.98</v>
+      </c>
+      <c r="I76">
+        <v>12</v>
+      </c>
+      <c r="J76">
+        <v>196.56</v>
+      </c>
+      <c r="K76">
+        <v>6</v>
+      </c>
+      <c r="L76">
+        <v>52</v>
+      </c>
+      <c r="M76">
+        <v>26</v>
+      </c>
+      <c r="N76">
+        <v>23.34</v>
+      </c>
+      <c r="O76" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="77" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
+        <v>33</v>
+      </c>
+      <c r="B77" t="s">
+        <v>28</v>
+      </c>
+      <c r="C77">
+        <v>658.05399999999997</v>
+      </c>
+      <c r="D77">
+        <v>2.19469</v>
+      </c>
+      <c r="E77">
+        <v>4</v>
+      </c>
+      <c r="F77">
+        <v>25.06</v>
+      </c>
+      <c r="G77">
+        <v>1</v>
+      </c>
+      <c r="H77">
+        <v>9.58</v>
+      </c>
+      <c r="I77">
+        <v>4</v>
+      </c>
+      <c r="J77">
+        <v>182.06</v>
+      </c>
+      <c r="K77">
+        <v>6</v>
+      </c>
+      <c r="L77">
+        <v>60.84</v>
+      </c>
+      <c r="M77">
+        <v>15</v>
+      </c>
+      <c r="N77">
+        <v>22.46</v>
+      </c>
+      <c r="O77" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="78" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A78" t="s">
+        <v>34</v>
+      </c>
+      <c r="B78" t="s">
+        <v>27</v>
+      </c>
+      <c r="C78">
+        <v>837.01400000000001</v>
+      </c>
+      <c r="D78">
+        <v>2.8027500000000001</v>
+      </c>
+      <c r="E78">
+        <v>2</v>
+      </c>
+      <c r="F78">
+        <v>1.96</v>
+      </c>
+      <c r="G78">
+        <v>0</v>
+      </c>
+      <c r="H78">
+        <v>0</v>
+      </c>
+      <c r="I78">
+        <v>8</v>
+      </c>
+      <c r="J78">
+        <v>130.06</v>
+      </c>
+      <c r="K78">
+        <v>18</v>
+      </c>
+      <c r="L78">
+        <v>121.68</v>
+      </c>
+      <c r="M78">
+        <v>26</v>
+      </c>
+      <c r="N78">
+        <v>45.24</v>
+      </c>
+      <c r="O78" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="79" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
+        <v>34</v>
+      </c>
+      <c r="B79" t="s">
+        <v>28</v>
+      </c>
+      <c r="C79">
+        <v>673.03200000000004</v>
+      </c>
+      <c r="D79">
+        <v>2.24464</v>
+      </c>
+      <c r="E79">
+        <v>12</v>
+      </c>
+      <c r="F79">
+        <v>8.68</v>
+      </c>
+      <c r="G79">
+        <v>3</v>
+      </c>
+      <c r="H79">
+        <v>5.6</v>
+      </c>
+      <c r="I79">
+        <v>6</v>
+      </c>
+      <c r="J79">
+        <v>125.84</v>
+      </c>
+      <c r="K79">
+        <v>8</v>
+      </c>
+      <c r="L79">
+        <v>102.86</v>
+      </c>
+      <c r="M79">
+        <v>28</v>
+      </c>
+      <c r="N79">
+        <v>57.02</v>
+      </c>
+      <c r="O79" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="80" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A80" t="s">
+        <v>35</v>
+      </c>
+      <c r="B80" t="s">
+        <v>27</v>
+      </c>
+      <c r="C80">
+        <v>883.68799999999999</v>
+      </c>
+      <c r="D80">
+        <v>2.9535</v>
+      </c>
+      <c r="E80">
+        <v>8</v>
+      </c>
+      <c r="F80">
+        <v>16.579999999999998</v>
+      </c>
+      <c r="G80">
+        <v>6</v>
+      </c>
+      <c r="H80">
+        <v>9.08</v>
+      </c>
+      <c r="I80">
+        <v>5</v>
+      </c>
+      <c r="J80">
+        <v>192.5</v>
+      </c>
+      <c r="K80">
+        <v>4</v>
+      </c>
+      <c r="L80">
+        <v>53.48</v>
+      </c>
+      <c r="M80">
+        <v>22</v>
+      </c>
+      <c r="N80">
+        <v>27.94</v>
+      </c>
+      <c r="O80" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="81" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A81" t="s">
+        <v>35</v>
+      </c>
+      <c r="B81" t="s">
+        <v>28</v>
+      </c>
+      <c r="C81">
+        <v>1420.64</v>
+      </c>
+      <c r="D81">
+        <v>4.7420999999999998</v>
+      </c>
+      <c r="E81">
+        <v>16</v>
+      </c>
+      <c r="F81">
+        <v>88.6</v>
+      </c>
+      <c r="G81">
+        <v>5</v>
+      </c>
+      <c r="H81">
+        <v>33.159999999999997</v>
+      </c>
+      <c r="I81">
+        <v>18</v>
+      </c>
+      <c r="J81">
+        <v>63.02</v>
+      </c>
+      <c r="K81">
+        <v>10</v>
+      </c>
+      <c r="L81">
+        <v>62.4</v>
+      </c>
+      <c r="M81">
+        <v>48</v>
+      </c>
+      <c r="N81">
+        <v>52.76</v>
+      </c>
+      <c r="O81" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="82" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A82" t="s">
+        <v>31</v>
+      </c>
+      <c r="B82" t="s">
+        <v>27</v>
+      </c>
+      <c r="C82">
+        <v>1287.24</v>
+      </c>
+      <c r="D82">
+        <v>4.2962499999999997</v>
+      </c>
+      <c r="E82">
+        <v>11</v>
+      </c>
+      <c r="F82">
+        <v>96.96</v>
+      </c>
+      <c r="G82">
+        <v>5</v>
+      </c>
+      <c r="H82">
+        <v>55.1</v>
+      </c>
+      <c r="I82">
+        <v>8</v>
+      </c>
+      <c r="J82">
+        <v>56.58</v>
+      </c>
+      <c r="K82">
+        <v>7</v>
+      </c>
+      <c r="L82">
+        <v>54.88</v>
+      </c>
+      <c r="M82">
+        <v>30</v>
+      </c>
+      <c r="N82">
+        <v>36.4</v>
+      </c>
+      <c r="O82" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="83" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A83" t="s">
+        <v>31</v>
+      </c>
+      <c r="B83" t="s">
+        <v>28</v>
+      </c>
+      <c r="C83">
+        <v>1084.01</v>
+      </c>
+      <c r="D83">
+        <v>3.6152899999999999</v>
+      </c>
+      <c r="E83">
+        <v>15</v>
+      </c>
+      <c r="F83">
+        <v>93.6</v>
+      </c>
+      <c r="G83">
+        <v>4</v>
+      </c>
+      <c r="H83">
+        <v>17.12</v>
+      </c>
+      <c r="I83">
+        <v>9</v>
+      </c>
+      <c r="J83">
+        <v>82.44</v>
+      </c>
+      <c r="K83">
+        <v>8</v>
+      </c>
+      <c r="L83">
+        <v>49.58</v>
+      </c>
+      <c r="M83">
+        <v>35</v>
+      </c>
+      <c r="N83">
+        <v>57.26</v>
+      </c>
+      <c r="O83" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="84" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A84" t="s">
+        <v>32</v>
+      </c>
+      <c r="B84" t="s">
+        <v>27</v>
+      </c>
+      <c r="C84">
+        <v>1531.85</v>
+      </c>
+      <c r="D84">
+        <v>5.1146799999999999</v>
+      </c>
+      <c r="E84">
+        <v>7</v>
+      </c>
+      <c r="F84">
+        <v>44.28</v>
+      </c>
+      <c r="G84">
+        <v>2</v>
+      </c>
+      <c r="H84">
+        <v>10.72</v>
+      </c>
+      <c r="I84">
+        <v>14</v>
+      </c>
+      <c r="J84">
+        <v>88.46</v>
+      </c>
+      <c r="K84">
+        <v>19</v>
+      </c>
+      <c r="L84">
+        <v>104</v>
+      </c>
+      <c r="M84">
+        <v>41</v>
+      </c>
+      <c r="N84">
+        <v>52.34</v>
+      </c>
+      <c r="O84" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="85" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A85" t="s">
+        <v>32</v>
+      </c>
+      <c r="B85" t="s">
+        <v>28</v>
+      </c>
+      <c r="C85">
+        <v>1210.67</v>
+      </c>
+      <c r="D85">
+        <v>4.0466100000000003</v>
+      </c>
+      <c r="E85">
+        <v>7</v>
+      </c>
+      <c r="F85">
+        <v>43.12</v>
+      </c>
+      <c r="G85">
+        <v>2</v>
+      </c>
+      <c r="H85">
+        <v>1.56</v>
+      </c>
+      <c r="I85">
+        <v>12</v>
+      </c>
+      <c r="J85">
+        <v>137.30000000000001</v>
+      </c>
+      <c r="K85">
+        <v>12</v>
+      </c>
+      <c r="L85">
+        <v>84.42</v>
+      </c>
+      <c r="M85">
+        <v>30</v>
+      </c>
+      <c r="N85">
+        <v>33.24</v>
+      </c>
+      <c r="O85" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="86" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A86" t="s">
+        <v>33</v>
+      </c>
+      <c r="B86" t="s">
+        <v>27</v>
+      </c>
+      <c r="C86">
+        <v>1161.6099999999999</v>
+      </c>
+      <c r="D86">
+        <v>3.8727299999999998</v>
+      </c>
+      <c r="E86">
+        <v>8</v>
+      </c>
+      <c r="F86">
+        <v>59.517299999999999</v>
+      </c>
+      <c r="G86">
+        <v>2</v>
+      </c>
+      <c r="H86">
+        <v>17.4251</v>
+      </c>
+      <c r="I86">
+        <v>8</v>
+      </c>
+      <c r="J86">
+        <v>46.193399999999997</v>
+      </c>
+      <c r="K86">
+        <v>12</v>
+      </c>
+      <c r="L86">
+        <v>136.13200000000001</v>
+      </c>
+      <c r="M86">
+        <v>29</v>
+      </c>
+      <c r="N86">
+        <v>40.7318</v>
+      </c>
+      <c r="O86" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="87" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A87" t="s">
+        <v>33</v>
+      </c>
+      <c r="B87" t="s">
+        <v>28</v>
+      </c>
+      <c r="C87">
+        <v>1089.3399999999999</v>
+      </c>
+      <c r="D87">
+        <v>3.6315400000000002</v>
+      </c>
+      <c r="E87">
+        <v>3</v>
+      </c>
+      <c r="F87">
+        <v>24.007000000000001</v>
+      </c>
+      <c r="G87">
+        <v>2</v>
+      </c>
+      <c r="H87">
+        <v>9.3226999999999993</v>
+      </c>
+      <c r="I87">
+        <v>8</v>
+      </c>
+      <c r="J87">
+        <v>54.6158</v>
+      </c>
+      <c r="K87">
+        <v>9</v>
+      </c>
+      <c r="L87">
+        <v>173.303</v>
+      </c>
+      <c r="M87">
+        <v>21</v>
+      </c>
+      <c r="N87">
+        <v>38.751199999999997</v>
+      </c>
+      <c r="O87" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="88" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A88" t="s">
+        <v>34</v>
+      </c>
+      <c r="B88" t="s">
+        <v>27</v>
+      </c>
+      <c r="C88">
+        <v>1369.96</v>
+      </c>
+      <c r="D88">
+        <v>4.5698699999999999</v>
+      </c>
+      <c r="E88">
+        <v>10</v>
+      </c>
+      <c r="F88">
+        <v>17.600000000000001</v>
+      </c>
+      <c r="G88">
+        <v>8</v>
+      </c>
+      <c r="H88">
+        <v>14.64</v>
+      </c>
+      <c r="I88">
+        <v>10</v>
+      </c>
+      <c r="J88">
+        <v>73.52</v>
+      </c>
+      <c r="K88">
+        <v>29</v>
+      </c>
+      <c r="L88">
+        <v>114.6</v>
+      </c>
+      <c r="M88">
+        <v>57</v>
+      </c>
+      <c r="N88">
+        <v>79.64</v>
+      </c>
+      <c r="O88" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="89" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A89" t="s">
+        <v>34</v>
+      </c>
+      <c r="B89" t="s">
+        <v>28</v>
+      </c>
+      <c r="C89">
+        <v>983.63900000000001</v>
+      </c>
+      <c r="D89">
+        <v>3.2860200000000002</v>
+      </c>
+      <c r="E89">
+        <v>10</v>
+      </c>
+      <c r="F89">
+        <v>42.28</v>
+      </c>
+      <c r="G89">
+        <v>8</v>
+      </c>
+      <c r="H89">
+        <v>15.9</v>
+      </c>
+      <c r="I89">
+        <v>13</v>
+      </c>
+      <c r="J89">
+        <v>75.78</v>
+      </c>
+      <c r="K89">
+        <v>11</v>
+      </c>
+      <c r="L89">
+        <v>99.96</v>
+      </c>
+      <c r="M89">
+        <v>39</v>
+      </c>
+      <c r="N89">
+        <v>65.7</v>
+      </c>
+      <c r="O89" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="90" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A90" t="s">
+        <v>35</v>
+      </c>
+      <c r="B90" t="s">
+        <v>27</v>
+      </c>
+      <c r="C90">
+        <v>945.61199999999997</v>
+      </c>
+      <c r="D90">
+        <v>3.2553000000000001</v>
+      </c>
+      <c r="E90">
+        <v>8</v>
+      </c>
+      <c r="F90">
+        <v>31.682200000000002</v>
+      </c>
+      <c r="G90">
+        <v>3</v>
+      </c>
+      <c r="H90">
+        <v>7.7422399999999998</v>
+      </c>
+      <c r="I90">
+        <v>5</v>
+      </c>
+      <c r="J90">
+        <v>31.949300000000001</v>
+      </c>
+      <c r="K90">
+        <v>20</v>
+      </c>
+      <c r="L90">
+        <v>196.23699999999999</v>
+      </c>
+      <c r="M90">
+        <v>31</v>
+      </c>
+      <c r="N90">
+        <v>23.326799999999999</v>
+      </c>
+      <c r="O90" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="91" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A91" t="s">
+        <v>35</v>
+      </c>
+      <c r="B91" t="s">
+        <v>28</v>
+      </c>
+      <c r="C91">
+        <v>1602.19</v>
+      </c>
+      <c r="D91">
+        <v>5.3415800000000004</v>
+      </c>
+      <c r="E91">
+        <v>20</v>
+      </c>
+      <c r="F91">
+        <v>108.538</v>
+      </c>
+      <c r="G91">
+        <v>6</v>
+      </c>
+      <c r="H91">
+        <v>37.750900000000001</v>
+      </c>
+      <c r="I91">
+        <v>21</v>
+      </c>
+      <c r="J91">
+        <v>53.461500000000001</v>
+      </c>
+      <c r="K91">
+        <v>10</v>
+      </c>
+      <c r="L91">
+        <v>43.672699999999999</v>
+      </c>
+      <c r="M91">
+        <v>55</v>
+      </c>
+      <c r="N91">
+        <v>56.5764</v>
+      </c>
+      <c r="O91" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>